<commit_message>
Renamed populationDataProcess1 file, made changes to .xlsx files in datapandas directory, committed populationDataProcess2 & populationDataProcess3
</commit_message>
<xml_diff>
--- a/datapandas/ABS2021AgeBySexGrp.xlsx
+++ b/datapandas/ABS2021AgeBySexGrp.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TAS" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="QLD" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="SA" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="WA" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="OTH" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ACT" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="NSW" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="VIC" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="NT" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="NSW" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="VIC" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="QLD" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="WA" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TAS" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="NT" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ACT" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="OTH" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6705</v>
+        <v>83254</v>
       </c>
       <c r="C2" t="n">
-        <v>7909</v>
+        <v>100154</v>
       </c>
     </row>
     <row r="3">
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3395</v>
+        <v>46132</v>
       </c>
       <c r="C3" t="n">
-        <v>4746</v>
+        <v>64569</v>
       </c>
     </row>
     <row r="4">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1381</v>
+        <v>20100</v>
       </c>
       <c r="C4" t="n">
-        <v>2419</v>
+        <v>35703</v>
       </c>
     </row>
     <row r="5">
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>263</v>
+        <v>4453</v>
       </c>
       <c r="C5" t="n">
-        <v>684</v>
+        <v>11033</v>
       </c>
     </row>
     <row r="6">
@@ -517,10 +517,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21</v>
+        <v>395</v>
       </c>
       <c r="C6" t="n">
-        <v>79</v>
+        <v>1518</v>
       </c>
     </row>
   </sheetData>
@@ -566,10 +566,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49551</v>
+        <v>64021</v>
       </c>
       <c r="C2" t="n">
-        <v>57067</v>
+        <v>77579</v>
       </c>
     </row>
     <row r="3">
@@ -579,10 +579,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25196</v>
+        <v>35507</v>
       </c>
       <c r="C3" t="n">
-        <v>34393</v>
+        <v>50516</v>
       </c>
     </row>
     <row r="4">
@@ -592,10 +592,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10431</v>
+        <v>15674</v>
       </c>
       <c r="C4" t="n">
-        <v>18464</v>
+        <v>27515</v>
       </c>
     </row>
     <row r="5">
@@ -605,10 +605,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2196</v>
+        <v>3543</v>
       </c>
       <c r="C5" t="n">
-        <v>5510</v>
+        <v>8292</v>
       </c>
     </row>
     <row r="6">
@@ -618,10 +618,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>187</v>
+        <v>292</v>
       </c>
       <c r="C6" t="n">
-        <v>761</v>
+        <v>1128</v>
       </c>
     </row>
   </sheetData>
@@ -667,10 +667,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20397</v>
+        <v>49551</v>
       </c>
       <c r="C2" t="n">
-        <v>25270</v>
+        <v>57067</v>
       </c>
     </row>
     <row r="3">
@@ -680,10 +680,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11593</v>
+        <v>25196</v>
       </c>
       <c r="C3" t="n">
-        <v>16220</v>
+        <v>34393</v>
       </c>
     </row>
     <row r="4">
@@ -693,10 +693,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5231</v>
+        <v>10431</v>
       </c>
       <c r="C4" t="n">
-        <v>9348</v>
+        <v>18464</v>
       </c>
     </row>
     <row r="5">
@@ -706,10 +706,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1249</v>
+        <v>2196</v>
       </c>
       <c r="C5" t="n">
-        <v>3103</v>
+        <v>5510</v>
       </c>
     </row>
     <row r="6">
@@ -719,10 +719,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="C6" t="n">
-        <v>428</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -768,10 +768,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24274</v>
+        <v>20397</v>
       </c>
       <c r="C2" t="n">
-        <v>28842</v>
+        <v>25270</v>
       </c>
     </row>
     <row r="3">
@@ -781,10 +781,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12900</v>
+        <v>11593</v>
       </c>
       <c r="C3" t="n">
-        <v>17997</v>
+        <v>16220</v>
       </c>
     </row>
     <row r="4">
@@ -794,10 +794,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5399</v>
+        <v>5231</v>
       </c>
       <c r="C4" t="n">
-        <v>9286</v>
+        <v>9348</v>
       </c>
     </row>
     <row r="5">
@@ -807,10 +807,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1245</v>
+        <v>1249</v>
       </c>
       <c r="C5" t="n">
-        <v>2762</v>
+        <v>3103</v>
       </c>
     </row>
     <row r="6">
@@ -820,10 +820,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="C6" t="n">
-        <v>412</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -869,10 +869,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49</v>
+        <v>24274</v>
       </c>
       <c r="C2" t="n">
-        <v>56</v>
+        <v>28842</v>
       </c>
     </row>
     <row r="3">
@@ -882,10 +882,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>19</v>
+        <v>12900</v>
       </c>
       <c r="C3" t="n">
-        <v>25</v>
+        <v>17997</v>
       </c>
     </row>
     <row r="4">
@@ -895,10 +895,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>5399</v>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>9286</v>
       </c>
     </row>
     <row r="5">
@@ -908,10 +908,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1245</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="6">
@@ -921,10 +921,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -970,10 +970,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3328</v>
+        <v>6705</v>
       </c>
       <c r="C2" t="n">
-        <v>4271</v>
+        <v>7909</v>
       </c>
     </row>
     <row r="3">
@@ -983,10 +983,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1859</v>
+        <v>3395</v>
       </c>
       <c r="C3" t="n">
-        <v>2576</v>
+        <v>4746</v>
       </c>
     </row>
     <row r="4">
@@ -996,10 +996,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>804</v>
+        <v>1381</v>
       </c>
       <c r="C4" t="n">
-        <v>1261</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="5">
@@ -1009,10 +1009,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>190</v>
+        <v>263</v>
       </c>
       <c r="C5" t="n">
-        <v>426</v>
+        <v>684</v>
       </c>
     </row>
     <row r="6">
@@ -1022,10 +1022,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1071,10 +1071,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>83254</v>
+        <v>903</v>
       </c>
       <c r="C2" t="n">
-        <v>100154</v>
+        <v>974</v>
       </c>
     </row>
     <row r="3">
@@ -1084,10 +1084,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>46132</v>
+        <v>338</v>
       </c>
       <c r="C3" t="n">
-        <v>64569</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4">
@@ -1097,10 +1097,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20100</v>
+        <v>131</v>
       </c>
       <c r="C4" t="n">
-        <v>35703</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5">
@@ -1110,10 +1110,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4453</v>
+        <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>11033</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>395</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1518</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1172,10 +1172,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>64021</v>
+        <v>3328</v>
       </c>
       <c r="C2" t="n">
-        <v>77579</v>
+        <v>4271</v>
       </c>
     </row>
     <row r="3">
@@ -1185,10 +1185,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>35507</v>
+        <v>1859</v>
       </c>
       <c r="C3" t="n">
-        <v>50516</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="4">
@@ -1198,10 +1198,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>15674</v>
+        <v>804</v>
       </c>
       <c r="C4" t="n">
-        <v>27515</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="5">
@@ -1211,10 +1211,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3543</v>
+        <v>190</v>
       </c>
       <c r="C5" t="n">
-        <v>8292</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6">
@@ -1224,10 +1224,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>292</v>
+        <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>1128</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1273,10 +1273,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>903</v>
+        <v>49</v>
       </c>
       <c r="C2" t="n">
-        <v>974</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
@@ -1286,10 +1286,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>338</v>
+        <v>19</v>
       </c>
       <c r="C3" t="n">
-        <v>421</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -1299,10 +1299,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>194</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -1312,10 +1312,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1325,10 +1325,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>